<commit_message>
all pkgs, items mapped
</commit_message>
<xml_diff>
--- a/admin/Arches_Import_roadmap.xlsx
+++ b/admin/Arches_Import_roadmap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tw/PycharmProjects/arches/OLD/digipolis-arches-pkg/admin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tw/PycharmProjects/arches/digipolis-arches-pkg/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA483B69-1107-D946-BEAC-C2F1882B33D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD09E920-C698-D344-AF29-0F94356E43A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="4" xr2:uid="{1F4FA750-7528-134A-A1E0-8995DC724E06}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t>Resource Model</t>
   </si>
@@ -230,30 +230,9 @@
     <t># records</t>
   </si>
   <si>
-    <t>2260</t>
-  </si>
-  <si>
-    <t>9709</t>
-  </si>
-  <si>
-    <t>8999</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
-    <t>23m4.452s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64m5.088s      </t>
-  </si>
-  <si>
-    <t>202m50.921s</t>
-  </si>
-  <si>
-    <t>47m37.664s</t>
-  </si>
-  <si>
     <t>method</t>
   </si>
   <si>
@@ -266,13 +245,19 @@
     <t>Total # records</t>
   </si>
   <si>
-    <t>151233</t>
-  </si>
-  <si>
-    <t>284068</t>
-  </si>
-  <si>
     <t>* bulk shaky for some reason, will test more</t>
+  </si>
+  <si>
+    <t>DIFF</t>
+  </si>
+  <si>
+    <t>Estimated time if linear</t>
+  </si>
+  <si>
+    <t>57h</t>
+  </si>
+  <si>
+    <t>44h</t>
   </si>
 </sst>
 </file>
@@ -311,7 +296,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,8 +333,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -409,11 +400,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -433,6 +433,14 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5304D455-B128-AC45-81CD-7270120E8F93}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1046,7 +1054,7 @@
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1077,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1091,8 +1099,11 @@
       <c r="G2" s="3">
         <v>57003</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1114,8 +1125,11 @@
       <c r="G3" s="3">
         <v>51494</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1138,7 +1152,7 @@
         <v>4542</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1160,8 +1174,11 @@
       <c r="G5" s="3">
         <v>19825</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1184,7 +1201,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1207,7 +1224,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1230,7 +1247,7 @@
         <v>4843</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1252,8 +1269,15 @@
       <c r="G9" s="3">
         <v>10528</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="20">
+        <f>SUM(D6:D9)</f>
+        <v>3567</v>
+      </c>
+      <c r="I9" s="20">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1276,7 +1300,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1298,8 +1322,15 @@
       <c r="G11" s="3">
         <v>816</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <f>SUM(C10:C11)</f>
+        <v>1431</v>
+      </c>
+      <c r="I11" s="19">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1324,11 +1355,24 @@
         <f>SUM(G2:G11)</f>
         <v>151233</v>
       </c>
+      <c r="I12" s="20">
+        <f>SUM(I1:I11)</f>
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14">
+        <f>I12-D12</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D12:E12" formulaRange="1"/>
+    <ignoredError sqref="E12" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1420,18 +1464,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD545B3A-1C81-344F-9A02-D45E73665599}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1470,104 +1514,113 @@
       <c r="A3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>49</v>
+      <c r="B3" s="22">
+        <v>2260</v>
+      </c>
+      <c r="C3" s="22">
+        <v>9709</v>
+      </c>
+      <c r="D3" s="22">
+        <v>8999</v>
+      </c>
+      <c r="E3" s="22">
+        <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="B4" s="22">
+        <v>23</v>
+      </c>
+      <c r="C4" s="22">
+        <v>64</v>
+      </c>
+      <c r="D4" s="22">
+        <v>203</v>
+      </c>
+      <c r="E4" s="22">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>60</v>
+        <v>52</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="A6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="22">
+        <v>2260</v>
+      </c>
+      <c r="C6" s="22">
+        <v>9709</v>
+      </c>
+      <c r="D6" s="22">
+        <v>151233</v>
+      </c>
+      <c r="E6" s="22">
+        <v>284068</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="22">
+        <v>23</v>
+      </c>
+      <c r="C7" s="22">
         <v>64</v>
+      </c>
+      <c r="D7" s="22">
+        <f>D6/D3*D4</f>
+        <v>3411.5233914879427</v>
+      </c>
+      <c r="E7" s="22">
+        <f>E6/E3*47</f>
+        <v>2670.2392</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="17" t="s">
+        <v>56</v>
+      </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B3:E7" numberStoredAsText="1"/>
+    <ignoredError sqref="B5:E5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>